<commit_message>
DCF for LittelFuse (LFUS)
Created DCF model for LittelFuse (LFUS)
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61329CA-472F-4636-B439-CF87C4D2ACDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9296BA4-0BC4-45ED-91D6-547CC3B85B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6885" yWindow="2550" windowWidth="26955" windowHeight="17250" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="6885" yWindow="2550" windowWidth="21915" windowHeight="13650" activeTab="2" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comm Ind Bld Spply" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="114">
   <si>
     <t>Ticker</t>
   </si>
@@ -221,9 +221,6 @@
     <t>Hubbel</t>
   </si>
   <si>
-    <t>Littelfuse</t>
-  </si>
-  <si>
     <t>nVent Electric</t>
   </si>
   <si>
@@ -269,9 +266,6 @@
     <t>Power cable</t>
   </si>
   <si>
-    <t>Electronics</t>
-  </si>
-  <si>
     <t>Harnesses and Racks</t>
   </si>
   <si>
@@ -387,6 +381,15 @@
   </si>
   <si>
     <t>Great margins, and great utilization of PP&amp;E, low growth</t>
+  </si>
+  <si>
+    <t>LFUS</t>
+  </si>
+  <si>
+    <t>LittelFuse</t>
+  </si>
+  <si>
+    <t>Vehicle components</t>
   </si>
 </sst>
 </file>
@@ -484,7 +487,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -540,6 +543,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -588,7 +592,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -605,26 +609,26 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="N3">
-            <v>207.35</v>
+            <v>60.73</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>8070.4677499999998</v>
+            <v>5961.5730000000003</v>
           </cell>
         </row>
         <row r="18">
           <cell r="N18">
-            <v>11376.312419838127</v>
+            <v>6053.073284927159</v>
           </cell>
         </row>
         <row r="19">
           <cell r="N19">
-            <v>351.06657675784993</v>
+            <v>86.349119613796859</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -660,7 +664,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -696,7 +700,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -732,7 +736,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -768,7 +772,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -804,7 +808,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -840,7 +844,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -876,7 +880,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -912,7 +916,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -929,22 +933,22 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="N3">
-            <v>60.73</v>
+            <v>260.32</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>5961.5730000000003</v>
+            <v>6531.1078800000005</v>
           </cell>
         </row>
         <row r="18">
           <cell r="N18">
-            <v>6053.073284927159</v>
+            <v>8831.5667844635373</v>
           </cell>
         </row>
         <row r="19">
           <cell r="N19">
-            <v>86.349119613796859</v>
+            <v>357.06180902658434</v>
           </cell>
         </row>
       </sheetData>
@@ -1253,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569CADF2-2E0D-4D7A-9853-86DF7D017A5C}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,7 +1279,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1287,25 +1291,25 @@
         <v>4</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H1" s="11" t="s">
+      <c r="J1" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="K1" s="13" t="s">
         <v>107</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>109</v>
       </c>
       <c r="L1" t="s">
         <v>40</v>
@@ -1322,13 +1326,13 @@
         <v>49</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E2" s="24">
         <v>44775</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G2" s="14">
         <f>[1]Main!$N$8</f>
@@ -1351,7 +1355,7 @@
         <v>4.733613984693994</v>
       </c>
       <c r="L2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1371,7 +1375,7 @@
         <v>44858</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="14">
         <f>[2]Main!$N$8</f>
@@ -1394,7 +1398,7 @@
         <v>4.3731421333760139</v>
       </c>
       <c r="L3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1402,10 +1406,10 @@
         <v>44773</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>23</v>
@@ -1414,7 +1418,7 @@
         <v>44771</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G4" s="14">
         <f>[3]Main!$N$8</f>
@@ -1442,10 +1446,10 @@
         <v>44773</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>5</v>
@@ -1454,7 +1458,7 @@
         <v>44776</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G5" s="14">
         <f>[4]Main!$N$8</f>
@@ -1482,10 +1486,10 @@
         <v>44773</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>23</v>
@@ -1494,7 +1498,7 @@
         <v>44865</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G6" s="14">
         <f>[5]Main!$N$8</f>
@@ -1522,10 +1526,10 @@
         <v>44774</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>23</v>
@@ -1534,7 +1538,7 @@
         <v>44867</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G7" s="14">
         <f>[6]Main!$N$8</f>
@@ -1562,10 +1566,10 @@
         <v>44774</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>5</v>
@@ -1574,7 +1578,7 @@
         <v>44782</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G8" s="14">
         <f>[7]Main!$N$8</f>
@@ -1602,10 +1606,10 @@
         <v>44774</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>23</v>
@@ -1614,7 +1618,7 @@
         <v>44804</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G9" s="14">
         <f>[8]Main!$N$8</f>
@@ -1642,10 +1646,10 @@
         <v>44775</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>23</v>
@@ -1654,27 +1658,27 @@
         <v>44865</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G10" s="14">
-        <f>[10]Main!$N$8</f>
-        <v>8070.4677499999998</v>
+        <f>[9]Main!$N$8</f>
+        <v>6531.1078800000005</v>
       </c>
       <c r="H10" s="15">
-        <f>[10]Main!$N$18</f>
-        <v>11376.312419838127</v>
+        <f>[9]Main!$N$18</f>
+        <v>8831.5667844635373</v>
       </c>
       <c r="I10" s="21">
-        <f>[10]Main!$N$3</f>
-        <v>207.35</v>
+        <f>[9]Main!$N$3</f>
+        <v>260.32</v>
       </c>
       <c r="J10" s="21">
-        <f>[10]Main!$N$19</f>
-        <v>351.06657675784993</v>
+        <f>[9]Main!$N$19</f>
+        <v>357.06180902658434</v>
       </c>
       <c r="K10" s="16">
         <f t="shared" si="0"/>
-        <v>1.6931110526059798</v>
+        <v>1.3716264944168115</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1682,10 +1686,10 @@
         <v>44775</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>23</v>
@@ -1694,22 +1698,22 @@
         <v>44777</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G11" s="14">
-        <f>[9]Main!$N$8</f>
+        <f>[10]Main!$N$8</f>
         <v>5961.5730000000003</v>
       </c>
       <c r="H11" s="15">
-        <f>[9]Main!$N$18</f>
+        <f>[10]Main!$N$18</f>
         <v>6053.073284927159</v>
       </c>
       <c r="I11" s="21">
-        <f>[9]Main!$N$3</f>
+        <f>[10]Main!$N$3</f>
         <v>60.73</v>
       </c>
       <c r="J11" s="21">
-        <f>[9]Main!$N$19</f>
+        <f>[10]Main!$N$19</f>
         <v>86.349119613796859</v>
       </c>
       <c r="K11" s="16">
@@ -1722,10 +1726,10 @@
         <v>44775</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>23</v>
@@ -1734,7 +1738,7 @@
         <v>44777</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G12" s="14">
         <f>[11]Main!$N$8</f>
@@ -1757,21 +1761,21 @@
         <v>0.82662603606246043</v>
       </c>
       <c r="L12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N12" s="2"/>
     </row>
     <row r="26" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P27" t="s">
         <v>52</v>
@@ -1779,7 +1783,7 @@
     </row>
     <row r="30" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P30" t="s">
         <v>53</v>
@@ -1787,7 +1791,7 @@
     </row>
     <row r="32" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P32" t="s">
         <v>54</v>
@@ -1795,7 +1799,7 @@
     </row>
     <row r="33" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P33" t="s">
         <v>55</v>
@@ -1803,7 +1807,7 @@
     </row>
     <row r="34" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P34" t="s">
         <v>56</v>
@@ -1811,34 +1815,34 @@
     </row>
     <row r="36" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1928,7 +1932,7 @@
         <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
         <v>47</v>
@@ -2085,80 +2089,249 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F73C4D65-549C-45C8-8E56-0FDC50A5308E}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="E1" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="E2" s="24"/>
+      <c r="I2" s="21"/>
+      <c r="K2" s="16"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="24"/>
+      <c r="I3" s="21"/>
+      <c r="K3" s="16"/>
+      <c r="L3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="24"/>
+      <c r="I4" s="21"/>
+      <c r="K4" s="16"/>
+      <c r="L4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H14" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" t="s">
-        <v>57</v>
-      </c>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>44776</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="24">
+        <v>44858</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="14">
+        <f>[9]Main!$N$8</f>
+        <v>6531.1078800000005</v>
+      </c>
+      <c r="H5" s="15">
+        <f>[9]Main!$N$18</f>
+        <v>8831.5667844635373</v>
+      </c>
+      <c r="I5" s="21">
+        <f>[9]Main!$N$3</f>
+        <v>260.32</v>
+      </c>
+      <c r="J5" s="21">
+        <f>[9]Main!$N$19</f>
+        <v>357.06180902658434</v>
+      </c>
+      <c r="K5" s="16">
+        <f t="shared" ref="K5" si="0">J5/I5</f>
+        <v>1.3716264944168115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="E6" s="24"/>
+      <c r="I6" s="21"/>
+      <c r="K6" s="16"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="E7" s="24"/>
+      <c r="I7" s="21"/>
+      <c r="K7" s="16"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="E8" s="24"/>
+      <c r="I8" s="21"/>
+      <c r="K8" s="16"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="E9" s="24"/>
+      <c r="I9" s="21"/>
+      <c r="K9" s="16"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="E10" s="24"/>
+      <c r="I10" s="21"/>
+      <c r="K10" s="16"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="E11" s="24"/>
+      <c r="I11" s="21"/>
+      <c r="K11" s="16"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="E12" s="24"/>
+      <c r="I12" s="21"/>
+      <c r="K12" s="16"/>
+      <c r="N12" s="2"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K4 K6:K1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{2EB6F67C-0D9B-4ECF-9716-4DBD14C41168}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{BFD78B41-26C5-4F62-86C3-CB6F80A7C7C7}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{2FECCCE6-9678-48B4-953C-D18796E68957}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{2EB6F67C-0D9B-4ECF-9716-4DBD14C41168}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{BFD78B41-26C5-4F62-86C3-CB6F80A7C7C7}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{2FECCCE6-9678-48B4-953C-D18796E68957}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{04E6DBBA-9A36-417F-9821-390225E2FD6D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
DCF for LiquidityServices (LQDT)
Created DCF model for Liquidity Services (LQDT)
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9296BA4-0BC4-45ED-91D6-547CC3B85B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA0A710-585B-4048-AF77-7E4E3B289967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6885" yWindow="2550" windowWidth="21915" windowHeight="13650" activeTab="2" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="20565" yWindow="6090" windowWidth="21915" windowHeight="13650" activeTab="1" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comm Ind Bld Spply" sheetId="1" r:id="rId1"/>
-    <sheet name="Clothing" sheetId="2" r:id="rId2"/>
-    <sheet name="Semiconductors" sheetId="3" r:id="rId3"/>
+    <sheet name="Semiconductors" sheetId="3" r:id="rId2"/>
+    <sheet name="Clothing" sheetId="2" r:id="rId3"/>
+    <sheet name="Etc." sheetId="4" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
@@ -29,6 +29,8 @@
     <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
     <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
+    <externalReference r:id="rId16"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="118">
   <si>
     <t>Ticker</t>
   </si>
@@ -390,13 +392,26 @@
   </si>
   <si>
     <t>Vehicle components</t>
+  </si>
+  <si>
+    <t>General electronics</t>
+  </si>
+  <si>
+    <t>LQDT</t>
+  </si>
+  <si>
+    <t>Liquidity Services</t>
+  </si>
+  <si>
+    <t>Reverse supply chain</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0\x"/>
   </numFmts>
@@ -487,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -544,6 +559,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -665,6 +683,42 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="O3">
+            <v>18.149999999999999</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="O8">
+            <v>506.71814999999992</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="O18">
+            <v>541.46267091390234</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="O19">
+            <v>16.629178185986376</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1258,7 +1312,7 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1889,210 +1943,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53CF7099-1451-4043-B0D3-3FB9C121746E}">
-  <dimension ref="A1:G10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{0DF8380E-F130-4DF6-8C1B-81195F64E711}"/>
-    <hyperlink ref="A5" r:id="rId2" xr:uid="{E1F53057-56EF-47B9-8FE1-1577EBD42A71}"/>
-    <hyperlink ref="A10" r:id="rId3" xr:uid="{E611340F-90AF-4D19-BAC0-62BACF486418}"/>
-    <hyperlink ref="A9" r:id="rId4" xr:uid="{34820F31-FD3D-4DA0-BA88-FE235039C846}"/>
-    <hyperlink ref="A2" r:id="rId5" xr:uid="{3154E5F3-A90E-40D1-A213-6B2AD19D0831}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{7F400EBC-E648-4E90-B4D3-A13DFCE215CA}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{D983D58E-4193-450D-97E9-A90CF2926C9E}"/>
-    <hyperlink ref="A3" r:id="rId8" xr:uid="{3B3A617F-B0BC-4F0B-B959-6C0C93FA9FBA}"/>
-    <hyperlink ref="A7" r:id="rId9" xr:uid="{63119635-1507-495B-829C-7F604EBE1405}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F73C4D65-549C-45C8-8E56-0FDC50A5308E}">
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,6 +2016,9 @@
         <v>23</v>
       </c>
       <c r="E2" s="24"/>
+      <c r="F2" s="8" t="s">
+        <v>114</v>
+      </c>
       <c r="I2" s="21"/>
       <c r="K2" s="16"/>
     </row>
@@ -2176,6 +2034,9 @@
         <v>23</v>
       </c>
       <c r="E3" s="24"/>
+      <c r="F3" s="8" t="s">
+        <v>114</v>
+      </c>
       <c r="I3" s="21"/>
       <c r="K3" s="16"/>
       <c r="L3" t="s">
@@ -2194,6 +2055,9 @@
         <v>5</v>
       </c>
       <c r="E4" s="24"/>
+      <c r="F4" s="8" t="s">
+        <v>114</v>
+      </c>
       <c r="I4" s="21"/>
       <c r="K4" s="16"/>
       <c r="L4" t="s">
@@ -2335,4 +2199,444 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53CF7099-1451-4043-B0D3-3FB9C121746E}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="A20:D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{0DF8380E-F130-4DF6-8C1B-81195F64E711}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{E1F53057-56EF-47B9-8FE1-1577EBD42A71}"/>
+    <hyperlink ref="A10" r:id="rId3" xr:uid="{E611340F-90AF-4D19-BAC0-62BACF486418}"/>
+    <hyperlink ref="A9" r:id="rId4" xr:uid="{34820F31-FD3D-4DA0-BA88-FE235039C846}"/>
+    <hyperlink ref="A2" r:id="rId5" xr:uid="{3154E5F3-A90E-40D1-A213-6B2AD19D0831}"/>
+    <hyperlink ref="A6" r:id="rId6" xr:uid="{7F400EBC-E648-4E90-B4D3-A13DFCE215CA}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{D983D58E-4193-450D-97E9-A90CF2926C9E}"/>
+    <hyperlink ref="A3" r:id="rId8" xr:uid="{3B3A617F-B0BC-4F0B-B959-6C0C93FA9FBA}"/>
+    <hyperlink ref="A7" r:id="rId9" xr:uid="{63119635-1507-495B-829C-7F604EBE1405}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A980134-2B0C-4B8F-8791-A493F6352A74}">
+  <dimension ref="A1:N12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44777</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="24">
+        <v>44869</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" s="14">
+        <f>[12]Main!$O$8</f>
+        <v>506.71814999999992</v>
+      </c>
+      <c r="H2" s="15">
+        <f>[12]Main!$O$18</f>
+        <v>541.46267091390234</v>
+      </c>
+      <c r="I2" s="26">
+        <f>[12]Main!$O$3</f>
+        <v>18.149999999999999</v>
+      </c>
+      <c r="J2" s="26">
+        <f>[12]Main!$O$19</f>
+        <v>16.629178185986376</v>
+      </c>
+      <c r="K2" s="16">
+        <f t="shared" ref="K2" si="0">J2/I2</f>
+        <v>0.91620816451715581</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="E3" s="24"/>
+      <c r="I3" s="21"/>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="E4" s="24"/>
+      <c r="I4" s="21"/>
+      <c r="K4" s="16"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="E5" s="24"/>
+      <c r="I5" s="21"/>
+      <c r="K5" s="16"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="E6" s="24"/>
+      <c r="I6" s="21"/>
+      <c r="K6" s="16"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="E7" s="24"/>
+      <c r="I7" s="21"/>
+      <c r="K7" s="16"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="E8" s="24"/>
+      <c r="I8" s="21"/>
+      <c r="K8" s="16"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="E9" s="24"/>
+      <c r="I9" s="21"/>
+      <c r="K9" s="16"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="E10" s="24"/>
+      <c r="I10" s="21"/>
+      <c r="K10" s="16"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="E11" s="24"/>
+      <c r="I11" s="21"/>
+      <c r="K11" s="16"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="E12" s="24"/>
+      <c r="I12" s="21"/>
+      <c r="K12" s="16"/>
+      <c r="N12" s="2"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E2:E1048576">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K1048576">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{2BA61AB2-B324-4A96-BC09-D9608FDE949E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
QuickDCF for DHI Group (DHX)
Quick DCF model for DHI Group (DHX) using only 3years and MRQ data. Some notes on job seek website as well.
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA0A710-585B-4048-AF77-7E4E3B289967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C8B91C-54B1-4EA5-9D6A-0B1F4F110099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20565" yWindow="6090" windowWidth="21915" windowHeight="13650" activeTab="1" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="3090" yWindow="285" windowWidth="21915" windowHeight="13650" activeTab="3" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comm Ind Bld Spply" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="125">
   <si>
     <t>Ticker</t>
   </si>
@@ -404,6 +404,27 @@
   </si>
   <si>
     <t>Reverse supply chain</t>
+  </si>
+  <si>
+    <t>Home builder + rentals</t>
+  </si>
+  <si>
+    <t>DHI</t>
+  </si>
+  <si>
+    <t>D R Horton Inc</t>
+  </si>
+  <si>
+    <t>DHX</t>
+  </si>
+  <si>
+    <t>DHI Group</t>
+  </si>
+  <si>
+    <t>Job Posting and AI</t>
+  </si>
+  <si>
+    <t>Quick NPV (3Y, 1Q) - poor brand value, will fall</t>
   </si>
 </sst>
 </file>
@@ -610,7 +631,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -663,26 +684,26 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="N3">
-            <v>20.86</v>
+            <v>4.43</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>3705.70046</v>
+            <v>217.09325999999999</v>
           </cell>
         </row>
         <row r="18">
           <cell r="N18">
-            <v>2666.8844433216959</v>
+            <v>42.225188935657137</v>
           </cell>
         </row>
         <row r="19">
           <cell r="N19">
-            <v>17.243419112262924</v>
+            <v>0.9450156424434254</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -718,7 +739,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1312,7 +1333,7 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,28 +1817,45 @@
       </c>
       <c r="G12" s="14">
         <f>[11]Main!$N$8</f>
-        <v>3705.70046</v>
+        <v>217.09325999999999</v>
       </c>
       <c r="H12" s="15">
         <f>[11]Main!$N$18</f>
-        <v>2666.8844433216959</v>
+        <v>42.225188935657137</v>
       </c>
       <c r="I12" s="21">
         <f>[11]Main!$N$3</f>
-        <v>20.86</v>
+        <v>4.43</v>
       </c>
       <c r="J12" s="21">
         <f>[11]Main!$N$19</f>
-        <v>17.243419112262924</v>
+        <v>0.9450156424434254</v>
       </c>
       <c r="K12" s="16">
         <f t="shared" si="0"/>
-        <v>0.82662603606246043</v>
+        <v>0.21332181544998316</v>
       </c>
       <c r="L12" t="s">
         <v>109</v>
       </c>
       <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>44777</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="26" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O26" t="s">
@@ -1946,8 +1984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F73C4D65-549C-45C8-8E56-0FDC50A5308E}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2404,8 +2442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A980134-2B0C-4B8F-8791-A493F6352A74}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2498,16 +2536,52 @@
         <v>16.629178185986376</v>
       </c>
       <c r="K2" s="16">
-        <f t="shared" ref="K2" si="0">J2/I2</f>
+        <f t="shared" ref="K2:K3" si="0">J2/I2</f>
         <v>0.91620816451715581</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="E3" s="24"/>
-      <c r="I3" s="21"/>
-      <c r="K3" s="16"/>
+      <c r="A3" s="5">
+        <v>44777</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="24">
+        <v>44868</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="14">
+        <f>+[11]Main!$N$8</f>
+        <v>217.09325999999999</v>
+      </c>
+      <c r="H3" s="15">
+        <f>+[11]Main!$N$18</f>
+        <v>42.225188935657137</v>
+      </c>
+      <c r="I3" s="21">
+        <f>+[11]Main!$N$3</f>
+        <v>4.43</v>
+      </c>
+      <c r="J3" s="21">
+        <f>+[11]Main!$N$19</f>
+        <v>0.9450156424434254</v>
+      </c>
+      <c r="K3" s="16">
+        <f t="shared" si="0"/>
+        <v>0.21332181544998316</v>
+      </c>
+      <c r="L3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -2586,7 +2660,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K1048576">
+  <conditionalFormatting sqref="K4:K1048576">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2622,7 +2696,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
+  <conditionalFormatting sqref="K2:K3">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2636,6 +2710,7 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{2BA61AB2-B324-4A96-BC09-D9608FDE949E}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{1252D7D6-1977-4A37-ADFC-E3118CFC39F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
DCF for D R Horton Inc (DHI)
Created DCF model for D R Horton Inc (DHI), 20Q1 to 22Q3; 2017-2021
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C8B91C-54B1-4EA5-9D6A-0B1F4F110099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019912AD-5B44-4824-B872-6F35B52EE01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="285" windowWidth="21915" windowHeight="13650" activeTab="3" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="16815" yWindow="945" windowWidth="15420" windowHeight="13650" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comm Ind Bld Spply" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,8 @@
     <externalReference r:id="rId14"/>
     <externalReference r:id="rId15"/>
     <externalReference r:id="rId16"/>
+    <externalReference r:id="rId17"/>
+    <externalReference r:id="rId18"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -631,7 +633,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -703,7 +705,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -740,6 +742,78 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="N3">
+            <v>76.150000000000006</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="N8">
+            <v>31004.120000000003</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="N18">
+            <v>59674.776053903901</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="N19">
+            <v>170.11053607156185</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="N3">
+            <v>20.86</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="N8">
+            <v>3705.70046</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="N18">
+            <v>2666.8844433216959</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="N19">
+            <v>17.243419112262924</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1027,7 +1101,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1332,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569CADF2-2E0D-4D7A-9853-86DF7D017A5C}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,7 +1586,7 @@
         <v>52.989005935204794</v>
       </c>
       <c r="K4" s="16">
-        <f t="shared" ref="K4:K12" si="0">J4/I4</f>
+        <f t="shared" ref="K4:K13" si="0">J4/I4</f>
         <v>1.5006798622261339</v>
       </c>
     </row>
@@ -1816,24 +1890,24 @@
         <v>102</v>
       </c>
       <c r="G12" s="14">
-        <f>[11]Main!$N$8</f>
-        <v>217.09325999999999</v>
+        <f>[14]Main!$N$8</f>
+        <v>3705.70046</v>
       </c>
       <c r="H12" s="15">
-        <f>[11]Main!$N$18</f>
-        <v>42.225188935657137</v>
+        <f>[14]Main!$N$18</f>
+        <v>2666.8844433216959</v>
       </c>
       <c r="I12" s="21">
-        <f>[11]Main!$N$3</f>
-        <v>4.43</v>
+        <f>[14]Main!$N$3</f>
+        <v>20.86</v>
       </c>
       <c r="J12" s="21">
-        <f>[11]Main!$N$19</f>
-        <v>0.9450156424434254</v>
+        <f>[14]Main!$N$19</f>
+        <v>17.243419112262924</v>
       </c>
       <c r="K12" s="16">
         <f t="shared" si="0"/>
-        <v>0.21332181544998316</v>
+        <v>0.82662603606246043</v>
       </c>
       <c r="L12" t="s">
         <v>109</v>
@@ -1844,7 +1918,7 @@
       <c r="A13" s="5">
         <v>44777</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>119</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -1853,8 +1927,31 @@
       <c r="D13" s="25" t="s">
         <v>96</v>
       </c>
+      <c r="E13" s="24">
+        <v>44870</v>
+      </c>
       <c r="F13" s="8" t="s">
         <v>118</v>
+      </c>
+      <c r="G13" s="14">
+        <f>[13]Main!$N$8</f>
+        <v>31004.120000000003</v>
+      </c>
+      <c r="H13" s="15">
+        <f>[13]Main!$N$18</f>
+        <v>59674.776053903901</v>
+      </c>
+      <c r="I13" s="21">
+        <f>[13]Main!$N$3</f>
+        <v>76.150000000000006</v>
+      </c>
+      <c r="J13" s="21">
+        <f>[13]Main!$N$19</f>
+        <v>170.11053607156185</v>
+      </c>
+      <c r="K13" s="16">
+        <f t="shared" si="0"/>
+        <v>2.2338875386941806</v>
       </c>
     </row>
     <row r="26" spans="15:16" x14ac:dyDescent="0.25">
@@ -1974,9 +2071,10 @@
     <hyperlink ref="B11" r:id="rId9" xr:uid="{EC971D85-AE4D-4BAC-8F79-E09E5BB1E48F}"/>
     <hyperlink ref="B10" r:id="rId10" xr:uid="{3F8536C2-23A7-4161-812E-20365E1D9978}"/>
     <hyperlink ref="B12" r:id="rId11" xr:uid="{EADEAE13-3EB5-4DD8-A227-962C1710AB1F}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{8891FA92-2D91-4B39-8F9A-15A7A99C6B0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId12"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -2442,7 +2540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A980134-2B0C-4B8F-8791-A493F6352A74}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
DCF for Bed Bath and Beyond (BBBY)
Created DCF for Bed Bath and Beyond (BBBY), 9Q, 5Y, with notes
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C470FC9B-FD91-4D80-A1AD-FF9A6809A837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851298A5-D3D6-4F65-8C07-7F23EB3E8F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16815" yWindow="945" windowWidth="15420" windowHeight="13650" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="13200" yWindow="0" windowWidth="19005" windowHeight="13650" activeTab="3" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comm Ind Bld Spply" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <externalReference r:id="rId16"/>
     <externalReference r:id="rId17"/>
     <externalReference r:id="rId18"/>
+    <externalReference r:id="rId19"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="129">
   <si>
     <t>Ticker</t>
   </si>
@@ -427,6 +428,18 @@
   </si>
   <si>
     <t>Quick NPV (3Y, 1Q) - poor brand value, will fall</t>
+  </si>
+  <si>
+    <t>TEAM</t>
+  </si>
+  <si>
+    <t>BBBY</t>
+  </si>
+  <si>
+    <t>Bed Bath and Beyond</t>
+  </si>
+  <si>
+    <t>Home décor and nursury</t>
   </si>
 </sst>
 </file>
@@ -525,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -585,6 +598,8 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -686,22 +701,22 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="N3">
-            <v>4.43</v>
+            <v>20.86</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>217.09325999999999</v>
+            <v>3705.70046</v>
           </cell>
         </row>
         <row r="18">
           <cell r="N18">
-            <v>42.225188935657137</v>
+            <v>2666.8844433216959</v>
           </cell>
         </row>
         <row r="19">
           <cell r="N19">
-            <v>0.9450156424434254</v>
+            <v>17.243419112262924</v>
           </cell>
         </row>
       </sheetData>
@@ -721,23 +736,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="O3">
-            <v>18.149999999999999</v>
+          <cell r="N3">
+            <v>76.150000000000006</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="O8">
-            <v>506.71814999999992</v>
+          <cell r="N8">
+            <v>31004.120000000003</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="O18">
-            <v>541.46267091390234</v>
+          <cell r="N18">
+            <v>59674.776053903901</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="O19">
-            <v>16.629178185986376</v>
+          <cell r="N19">
+            <v>170.11053607156185</v>
           </cell>
         </row>
       </sheetData>
@@ -757,23 +772,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>76.150000000000006</v>
+          <cell r="J3">
+            <v>8.1999999999999993</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="N8">
-            <v>31004.120000000003</v>
+          <cell r="J8">
+            <v>3802.98</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="N18">
-            <v>59674.776053903901</v>
+          <cell r="J18">
+            <v>218.76521315251679</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="N19">
-            <v>170.11053607156185</v>
+          <cell r="J19">
+            <v>2.7483066978959396</v>
           </cell>
         </row>
       </sheetData>
@@ -794,22 +809,58 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="N3">
-            <v>20.86</v>
+            <v>4.43</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>3705.70046</v>
+            <v>217.09325999999999</v>
           </cell>
         </row>
         <row r="18">
           <cell r="N18">
-            <v>2666.8844433216959</v>
+            <v>42.225188935657137</v>
           </cell>
         </row>
         <row r="19">
           <cell r="N19">
-            <v>17.243419112262924</v>
+            <v>0.9450156424434254</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="O3">
+            <v>18.149999999999999</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="O8">
+            <v>506.71814999999992</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="O18">
+            <v>541.46267091390234</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="O19">
+            <v>16.629178185986376</v>
           </cell>
         </row>
       </sheetData>
@@ -1406,8 +1457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569CADF2-2E0D-4D7A-9853-86DF7D017A5C}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,19 +1941,19 @@
         <v>102</v>
       </c>
       <c r="G12" s="14">
-        <f>[14]Main!$N$8</f>
+        <f>[11]Main!$N$8</f>
         <v>3705.70046</v>
       </c>
       <c r="H12" s="15">
-        <f>[14]Main!$N$18</f>
+        <f>[11]Main!$N$18</f>
         <v>2666.8844433216959</v>
       </c>
       <c r="I12" s="21">
-        <f>[14]Main!$N$3</f>
+        <f>[11]Main!$N$3</f>
         <v>20.86</v>
       </c>
       <c r="J12" s="21">
-        <f>[14]Main!$N$19</f>
+        <f>[11]Main!$N$19</f>
         <v>17.243419112262924</v>
       </c>
       <c r="K12" s="16">
@@ -1934,19 +1985,19 @@
         <v>118</v>
       </c>
       <c r="G13" s="14">
-        <f>[13]Main!$N$8</f>
+        <f>[12]Main!$N$8</f>
         <v>31004.120000000003</v>
       </c>
       <c r="H13" s="15">
-        <f>[13]Main!$N$18</f>
+        <f>[12]Main!$N$18</f>
         <v>59674.776053903901</v>
       </c>
       <c r="I13" s="21">
-        <f>[13]Main!$N$3</f>
+        <f>[12]Main!$N$3</f>
         <v>76.150000000000006</v>
       </c>
       <c r="J13" s="21">
-        <f>[13]Main!$N$19</f>
+        <f>[12]Main!$N$19</f>
         <v>170.11053607156185</v>
       </c>
       <c r="K13" s="16">
@@ -2540,8 +2591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A980134-2B0C-4B8F-8791-A493F6352A74}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2618,23 +2669,23 @@
         <v>117</v>
       </c>
       <c r="G2" s="14">
-        <f>[12]Main!$O$8</f>
+        <f>[15]Main!$O$8</f>
         <v>506.71814999999992</v>
       </c>
       <c r="H2" s="15">
-        <f>[12]Main!$O$18</f>
+        <f>[15]Main!$O$18</f>
         <v>541.46267091390234</v>
       </c>
       <c r="I2" s="26">
-        <f>[12]Main!$O$3</f>
+        <f>[15]Main!$O$3</f>
         <v>18.149999999999999</v>
       </c>
-      <c r="J2" s="26">
-        <f>[12]Main!$O$19</f>
+      <c r="J2" s="27">
+        <f>[15]Main!$O$19</f>
         <v>16.629178185986376</v>
       </c>
       <c r="K2" s="16">
-        <f t="shared" ref="K2:K3" si="0">J2/I2</f>
+        <f t="shared" ref="K2:K4" si="0">J2/I2</f>
         <v>0.91620816451715581</v>
       </c>
     </row>
@@ -2658,19 +2709,19 @@
         <v>123</v>
       </c>
       <c r="G3" s="14">
-        <f>+[11]Main!$N$8</f>
+        <f>+[14]Main!$N$8</f>
         <v>217.09325999999999</v>
       </c>
       <c r="H3" s="15">
-        <f>+[11]Main!$N$18</f>
+        <f>+[14]Main!$N$18</f>
         <v>42.225188935657137</v>
       </c>
       <c r="I3" s="21">
-        <f>+[11]Main!$N$3</f>
+        <f>+[14]Main!$N$3</f>
         <v>4.43</v>
       </c>
-      <c r="J3" s="21">
-        <f>+[11]Main!$N$19</f>
+      <c r="J3" s="28">
+        <f>+[14]Main!$N$19</f>
         <v>0.9450156424434254</v>
       </c>
       <c r="K3" s="16">
@@ -2682,11 +2733,44 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="E4" s="24"/>
-      <c r="I4" s="21"/>
-      <c r="K4" s="16"/>
+      <c r="A4" s="5">
+        <v>44779</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="24">
+        <v>44832</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" s="14">
+        <f>[13]Main!$J$8</f>
+        <v>3802.98</v>
+      </c>
+      <c r="H4" s="15">
+        <f>[13]Main!$J$18</f>
+        <v>218.76521315251679</v>
+      </c>
+      <c r="I4" s="26">
+        <f>[13]Main!$J$3</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J4" s="28">
+        <f>[13]Main!$J$19</f>
+        <v>2.7483066978959396</v>
+      </c>
+      <c r="K4" s="16">
+        <f t="shared" si="0"/>
+        <v>0.33515935340194386</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
@@ -2697,7 +2781,9 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="E6" s="24"/>
       <c r="I6" s="21"/>
       <c r="K6" s="16"/>
@@ -2758,7 +2844,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4:K1048576">
+  <conditionalFormatting sqref="K5:K1048576">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2794,7 +2880,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K3">
+  <conditionalFormatting sqref="K2:K4">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>